<commit_message>
update the d3 branch
</commit_message>
<xml_diff>
--- a/data/EdNext_SchoolChoice.xlsx
+++ b/data/EdNext_SchoolChoice.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah Pollnow\OneDrive - Harvard University\J-Term\School Choice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sarah Pollnow\Desktop\Development\ed-elect\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -217,15 +217,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -238,6 +229,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -665,11 +665,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="683563776"/>
-        <c:axId val="683564952"/>
+        <c:axId val="319818968"/>
+        <c:axId val="319819360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="683563776"/>
+        <c:axId val="319818968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -712,7 +712,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="683564952"/>
+        <c:crossAx val="319819360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -720,7 +720,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="683564952"/>
+        <c:axId val="319819360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -829,7 +829,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="683563776"/>
+        <c:crossAx val="319818968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1228,11 +1228,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="691801304"/>
-        <c:axId val="691802088"/>
+        <c:axId val="322031920"/>
+        <c:axId val="322029176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="691801304"/>
+        <c:axId val="322031920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1275,7 +1275,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="691802088"/>
+        <c:crossAx val="322029176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1283,7 +1283,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="691802088"/>
+        <c:axId val="322029176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1334,7 +1334,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="691801304"/>
+        <c:crossAx val="322031920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1815,11 +1815,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="687663568"/>
-        <c:axId val="687660040"/>
+        <c:axId val="322027216"/>
+        <c:axId val="322026040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="687663568"/>
+        <c:axId val="322027216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1862,7 +1862,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="687660040"/>
+        <c:crossAx val="322026040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1870,7 +1870,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="687660040"/>
+        <c:axId val="322026040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1979,7 +1979,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="687663568"/>
+        <c:crossAx val="322027216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2378,11 +2378,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="694469056"/>
-        <c:axId val="694471800"/>
+        <c:axId val="322032312"/>
+        <c:axId val="322030352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="694469056"/>
+        <c:axId val="322032312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2425,7 +2425,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="694471800"/>
+        <c:crossAx val="322030352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2433,7 +2433,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="694471800"/>
+        <c:axId val="322030352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="70"/>
@@ -2541,7 +2541,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="694469056"/>
+        <c:crossAx val="322032312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3183,11 +3183,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="515661712"/>
-        <c:axId val="515658968"/>
+        <c:axId val="322026824"/>
+        <c:axId val="322031136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="515661712"/>
+        <c:axId val="322026824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3230,7 +3230,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="515658968"/>
+        <c:crossAx val="322031136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3238,7 +3238,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="515658968"/>
+        <c:axId val="322031136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3347,7 +3347,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="515661712"/>
+        <c:crossAx val="322026824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6388,16 +6388,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>373178</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>44954</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>614869</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>90271</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>108134</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>261360</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>349825</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>306676</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6684,8 +6684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:G22"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6727,7 +6727,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -6753,7 +6753,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A6" s="4"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -6777,7 +6777,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A7" s="6"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -6801,7 +6801,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -6827,7 +6827,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A9" s="4"/>
+      <c r="A9" s="11"/>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
@@ -6851,7 +6851,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="6"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
@@ -6875,7 +6875,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -6901,7 +6901,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A12" s="4"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
@@ -6925,7 +6925,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A13" s="6"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
@@ -6949,7 +6949,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -6975,7 +6975,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A15" s="4"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
@@ -6999,7 +6999,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A16" s="6"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="3" t="s">
         <v>5</v>
       </c>
@@ -7049,7 +7049,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="3">
@@ -7072,7 +7072,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="3">
@@ -7095,7 +7095,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="3">
@@ -7134,8 +7134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:G22"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7177,7 +7177,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="3"/>
@@ -7196,7 +7196,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="29.1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="3"/>
@@ -7215,7 +7215,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="3"/>
@@ -7243,8 +7243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C33:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7253,269 +7253,269 @@
   </cols>
   <sheetData>
     <row r="33" spans="3:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="10"/>
-      <c r="T33" s="10"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
     </row>
     <row r="34" spans="3:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
-      <c r="S34" s="10"/>
-      <c r="T34" s="10"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
     </row>
     <row r="35" spans="3:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
-      <c r="S35" s="10"/>
-      <c r="T35" s="10"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
     </row>
     <row r="36" spans="3:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="C36" s="12"/>
-      <c r="D36" s="12">
+      <c r="C36" s="9"/>
+      <c r="D36" s="9">
         <v>2013</v>
       </c>
-      <c r="E36" s="12">
+      <c r="E36" s="9">
         <v>2014</v>
       </c>
-      <c r="F36" s="12">
+      <c r="F36" s="9">
         <v>2015</v>
       </c>
-      <c r="G36" s="12">
+      <c r="G36" s="9">
         <v>2016</v>
       </c>
-      <c r="H36" s="12">
+      <c r="H36" s="9">
         <v>2017</v>
       </c>
-      <c r="I36" s="12">
+      <c r="I36" s="9">
         <v>2018</v>
       </c>
-      <c r="K36" s="10"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="10"/>
-      <c r="T36" s="10"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+      <c r="R36" s="8"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
     </row>
     <row r="37" spans="3:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="12">
+      <c r="D37" s="9">
         <v>60</v>
       </c>
-      <c r="E37" s="12">
+      <c r="E37" s="9">
         <v>64</v>
       </c>
-      <c r="F37" s="12">
+      <c r="F37" s="9">
         <v>62</v>
       </c>
-      <c r="G37" s="12">
+      <c r="G37" s="9">
         <v>60</v>
       </c>
-      <c r="H37" s="12">
+      <c r="H37" s="9">
         <v>47</v>
       </c>
-      <c r="I37" s="12">
+      <c r="I37" s="9">
         <v>57</v>
       </c>
-      <c r="K37" s="10"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="10"/>
-      <c r="T37" s="10"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
     </row>
     <row r="38" spans="3:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12">
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9">
         <v>36</v>
       </c>
-      <c r="G38" s="12">
+      <c r="G38" s="9">
         <v>31</v>
       </c>
-      <c r="H38" s="12">
+      <c r="H38" s="9">
         <v>42</v>
       </c>
-      <c r="I38" s="12">
+      <c r="I38" s="9">
         <v>39</v>
       </c>
-      <c r="K38" s="10"/>
-      <c r="L38" s="11"/>
-      <c r="M38" s="11"/>
-      <c r="N38" s="11"/>
-      <c r="O38" s="11"/>
-      <c r="P38" s="11"/>
-      <c r="Q38" s="11"/>
-      <c r="R38" s="11"/>
-      <c r="S38" s="10"/>
-      <c r="T38" s="10"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="8"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
     </row>
     <row r="39" spans="3:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="12">
+      <c r="D39" s="9">
         <v>44</v>
       </c>
-      <c r="E39" s="12">
+      <c r="E39" s="9">
         <v>47</v>
       </c>
-      <c r="F39" s="12">
+      <c r="F39" s="9">
         <v>42</v>
       </c>
-      <c r="G39" s="12">
+      <c r="G39" s="9">
         <v>45</v>
       </c>
-      <c r="H39" s="12">
+      <c r="H39" s="9">
         <v>34</v>
       </c>
-      <c r="I39" s="12">
+      <c r="I39" s="9">
         <v>36</v>
       </c>
-      <c r="K39" s="10"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
-      <c r="S39" s="10"/>
-      <c r="T39" s="10"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="8"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="8"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
     </row>
     <row r="40" spans="3:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12">
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9">
         <v>47</v>
       </c>
-      <c r="G40" s="12">
+      <c r="G40" s="9">
         <v>42</v>
       </c>
-      <c r="H40" s="12">
+      <c r="H40" s="9">
         <v>44</v>
       </c>
-      <c r="I40" s="12">
+      <c r="I40" s="9">
         <v>47</v>
       </c>
-      <c r="K40" s="10"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="11"/>
-      <c r="S40" s="10"/>
-      <c r="T40" s="10"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="8"/>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="8"/>
+      <c r="R40" s="8"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
     </row>
     <row r="41" spans="3:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D41" s="12">
+      <c r="D41" s="9">
         <v>41</v>
       </c>
-      <c r="E41" s="12">
+      <c r="E41" s="9">
         <v>43</v>
       </c>
-      <c r="F41" s="12">
+      <c r="F41" s="9">
         <v>39</v>
       </c>
-      <c r="G41" s="12">
+      <c r="G41" s="9">
         <v>41</v>
       </c>
-      <c r="H41" s="12">
+      <c r="H41" s="9">
         <v>40</v>
       </c>
-      <c r="I41" s="12">
+      <c r="I41" s="9">
         <v>33</v>
       </c>
-      <c r="K41" s="10"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="10"/>
-      <c r="T41" s="10"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="8"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
     </row>
     <row r="42" spans="3:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="12">
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="9">
         <v>29</v>
       </c>
-      <c r="G42" s="12">
+      <c r="G42" s="9">
         <v>29</v>
       </c>
-      <c r="H42" s="12">
+      <c r="H42" s="9">
         <v>27</v>
       </c>
-      <c r="I42" s="12">
+      <c r="I42" s="9">
         <v>29</v>
       </c>
-      <c r="K42" s="10"/>
-      <c r="L42" s="10"/>
-      <c r="M42" s="10"/>
-      <c r="N42" s="10"/>
-      <c r="O42" s="10"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="10"/>
-      <c r="R42" s="10"/>
-      <c r="S42" s="10"/>
-      <c r="T42" s="10"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="7"/>
     </row>
     <row r="43" spans="3:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="K43" s="10"/>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-      <c r="S43" s="10"/>
-      <c r="T43" s="10"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>